<commit_message>
Adição da comparação entre RVND e ILS
</commit_message>
<xml_diff>
--- a/Arquivos/Resultados/Resultados ILS.xlsx
+++ b/Arquivos/Resultados/Resultados ILS.xlsx
@@ -228,11 +228,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="0_ "/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -251,7 +251,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,47 +264,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,7 +280,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,8 +317,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,24 +357,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -381,7 +373,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,7 +403,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,73 +529,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,97 +583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,41 +608,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -671,26 +636,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,157 +674,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -869,10 +869,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1197,7 +1200,7 @@
   <dimension ref="B2:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1284,7 +1287,7 @@
       <c r="K4" s="4">
         <v>210</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="5">
         <v>1902.27</v>
       </c>
     </row>
@@ -1313,7 +1316,7 @@
       <c r="K5" s="4">
         <v>36</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="5">
         <v>6252</v>
       </c>
     </row>
@@ -1342,7 +1345,7 @@
       <c r="K6" s="4">
         <v>21</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="5">
         <v>1040</v>
       </c>
     </row>
@@ -1371,7 +1374,7 @@
       <c r="K7" s="4">
         <v>21</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="5">
         <v>1159</v>
       </c>
     </row>
@@ -1400,7 +1403,7 @@
       <c r="K8" s="4">
         <v>39</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="5">
         <v>3910.64</v>
       </c>
     </row>
@@ -1429,7 +1432,7 @@
       <c r="K9" s="4">
         <v>95</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="5">
         <v>50282.14</v>
       </c>
     </row>
@@ -1458,7 +1461,7 @@
       <c r="K10" s="4">
         <v>43</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="5">
         <v>10035</v>
       </c>
     </row>
@@ -1487,7 +1490,7 @@
       <c r="K11" s="4">
         <v>135</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="5">
         <v>1460</v>
       </c>
     </row>
@@ -1516,7 +1519,7 @@
       <c r="K12" s="4">
         <v>10</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="5">
         <v>1637.31</v>
       </c>
     </row>
@@ -1545,7 +1548,7 @@
       <c r="K13" s="4">
         <v>97</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="5">
         <v>3884.41</v>
       </c>
     </row>
@@ -1574,7 +1577,7 @@
       <c r="K14" s="4">
         <v>112</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="5">
         <v>4599.97</v>
       </c>
     </row>
@@ -1603,7 +1606,7 @@
       <c r="K15" s="4">
         <v>31</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="5">
         <v>401</v>
       </c>
     </row>
@@ -1632,7 +1635,7 @@
       <c r="K16" s="4">
         <v>38</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="5">
         <v>281.61</v>
       </c>
     </row>
@@ -1661,7 +1664,7 @@
       <c r="K17" s="4">
         <v>57</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="5">
         <v>340.02</v>
       </c>
     </row>
@@ -1690,7 +1693,7 @@
       <c r="K18" s="4">
         <v>75</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="5">
         <v>438.75</v>
       </c>
     </row>
@@ -1719,7 +1722,7 @@
       <c r="K19" s="4">
         <v>19</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="5">
         <v>559</v>
       </c>
     </row>
@@ -1748,7 +1751,7 @@
       <c r="K20" s="4">
         <v>196</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="5">
         <v>1644.53</v>
       </c>
     </row>
@@ -1777,7 +1780,7 @@
       <c r="K21" s="4">
         <v>12</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="5">
         <v>640</v>
       </c>
     </row>
@@ -1806,7 +1809,7 @@
       <c r="K22" s="4">
         <v>15</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="5">
         <v>1331</v>
       </c>
     </row>
@@ -1835,7 +1838,7 @@
       <c r="K23" s="4">
         <v>18</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="5">
         <v>794</v>
       </c>
     </row>
@@ -1864,7 +1867,7 @@
       <c r="K24" s="4">
         <v>36</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="5">
         <v>3054</v>
       </c>
     </row>
@@ -1893,7 +1896,7 @@
       <c r="K25" s="4">
         <v>72</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="5">
         <v>36699.98</v>
       </c>
     </row>
@@ -1922,7 +1925,7 @@
       <c r="K26" s="4">
         <v>90</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="5">
         <v>4542</v>
       </c>
     </row>
@@ -1951,7 +1954,7 @@
       <c r="K27" s="4">
         <v>36</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="5">
         <v>7650</v>
       </c>
     </row>
@@ -1980,7 +1983,7 @@
       <c r="K28" s="4">
         <v>75</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="5">
         <v>14896.93</v>
       </c>
     </row>
@@ -2009,7 +2012,7 @@
       <c r="K29" s="4">
         <v>112</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="5">
         <v>19154.06</v>
       </c>
     </row>
@@ -2038,7 +2041,7 @@
       <c r="K30" s="4">
         <v>150</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="5">
         <v>20456.35</v>
       </c>
     </row>
@@ -2067,7 +2070,7 @@
       <c r="K31" s="4">
         <v>75</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="5">
         <v>15454.66</v>
       </c>
     </row>
@@ -2096,7 +2099,7 @@
       <c r="K32" s="4">
         <v>112</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="5">
         <v>16728.79</v>
       </c>
     </row>
@@ -2125,7 +2128,7 @@
       <c r="K33" s="4">
         <v>150</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="5">
         <v>20134.61</v>
       </c>
     </row>
@@ -2154,7 +2157,7 @@
       <c r="K34" s="4">
         <v>75</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="5">
         <v>13951.85</v>
       </c>
     </row>
@@ -2183,7 +2186,7 @@
       <c r="K35" s="4">
         <v>75</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="5">
         <v>14779.43</v>
       </c>
     </row>
@@ -2212,7 +2215,7 @@
       <c r="K36" s="4">
         <v>75</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="5">
         <v>14943.31</v>
       </c>
     </row>
@@ -2241,7 +2244,7 @@
       <c r="K37" s="4">
         <v>78</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="5">
         <v>8397.36</v>
       </c>
     </row>
@@ -2270,7 +2273,7 @@
       <c r="K38" s="4">
         <v>238</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="5">
         <v>29009.41</v>
       </c>
     </row>
@@ -2299,7 +2302,7 @@
       <c r="K39" s="4">
         <v>57</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="5">
         <v>61124.81</v>
       </c>
     </row>
@@ -2328,7 +2331,7 @@
       <c r="K40" s="4">
         <v>80</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="5">
         <v>30115.85</v>
       </c>
     </row>
@@ -2357,7 +2360,7 @@
       <c r="K41" s="4">
         <v>93</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="5">
         <v>37505.48</v>
       </c>
     </row>
@@ -2386,7 +2389,7 @@
       <c r="K42" s="4">
         <v>102</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="5">
         <v>72009.34</v>
       </c>
     </row>
@@ -2415,7 +2418,7 @@
       <c r="K43" s="4">
         <v>108</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="5">
         <v>40210.94</v>
       </c>
     </row>
@@ -2444,7 +2447,7 @@
       <c r="K44" s="4">
         <v>114</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="5">
         <v>46089.98</v>
       </c>
     </row>
@@ -2473,7 +2476,7 @@
       <c r="K45" s="4">
         <v>169</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="5">
         <v>48353.82</v>
       </c>
     </row>
@@ -2502,7 +2505,7 @@
       <c r="K46" s="4">
         <v>198</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46" s="5">
         <v>33977.04</v>
       </c>
     </row>
@@ -2531,7 +2534,7 @@
       <c r="K47" s="4">
         <v>224</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47" s="5">
         <v>34504.73</v>
       </c>
     </row>
@@ -2560,7 +2563,7 @@
       <c r="K48" s="4">
         <v>329</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48" s="5">
         <v>61894.86</v>
       </c>
     </row>
@@ -2589,7 +2592,7 @@
       <c r="K49" s="4">
         <v>74</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="5">
         <v>856.88</v>
       </c>
     </row>
@@ -2618,7 +2621,7 @@
       <c r="K50" s="4">
         <v>146</v>
       </c>
-      <c r="L50" s="4">
+      <c r="L50" s="5">
         <v>1669.63</v>
       </c>
     </row>
@@ -2647,7 +2650,7 @@
       <c r="K51" s="4">
         <v>131</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51" s="5">
         <v>15589</v>
       </c>
     </row>
@@ -2676,7 +2679,7 @@
       <c r="K52" s="4">
         <v>52</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52" s="5">
         <v>440.07</v>
       </c>
     </row>
@@ -2705,7 +2708,7 @@
       <c r="K53" s="4">
         <v>31</v>
       </c>
-      <c r="L53" s="4">
+      <c r="L53" s="5">
         <v>715</v>
       </c>
     </row>
@@ -2734,7 +2737,7 @@
       <c r="K54" s="4">
         <v>168</v>
       </c>
-      <c r="L54" s="4">
+      <c r="L54" s="5">
         <v>85571.07</v>
       </c>
     </row>
@@ -2763,7 +2766,7 @@
       <c r="K55" s="4">
         <v>168</v>
       </c>
-      <c r="L55" s="4">
+      <c r="L55" s="5">
         <v>2654.69</v>
       </c>
     </row>
@@ -2792,7 +2795,7 @@
       <c r="K56" s="4">
         <v>12</v>
       </c>
-      <c r="L56" s="4">
+      <c r="L56" s="5">
         <v>2741.1</v>
       </c>
     </row>
@@ -2821,7 +2824,7 @@
       <c r="K57" s="4">
         <v>16</v>
       </c>
-      <c r="L57" s="4">
+      <c r="L57" s="5">
         <v>2732.27</v>
       </c>
     </row>

</xml_diff>